<commit_message>
Modified all images extensions to be png to enhance model response Enhance handling of restore popup by putting it before navigating Reduces the delays when sending Instagram DMs to 2 seconds
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LLM VISION Uipath3\LLM VISION Uipath3 Github\Instagram-Facebook-Outreaching-Automation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679B283B-942C-466B-B0E2-B5BAD70FB679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA4A47C-73C2-41AC-A0FB-B403F5F75D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>meta-llama/llama-3.2-11b-vision-instruct:free</t>
+  </si>
+  <si>
+    <t>SplitterWord</t>
+  </si>
+  <si>
+    <t>I’m Visuals</t>
   </si>
 </sst>
 </file>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,6 +553,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhanced sending message to handle more dynamic cases
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LLM VISION Uipath3\LLM VISION Uipath3 Github\Instagram-Facebook-Outreaching-Automation\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UIPATH COMMAND ENTER\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA4A47C-73C2-41AC-A0FB-B403F5F75D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06E661A-7F1A-4246-A00C-3C15F61880BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -112,7 +112,7 @@
     <t>SplitterWord</t>
   </si>
   <si>
-    <t>I’m Visuals</t>
+    <t>I’m Visuals,</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>